<commit_message>
date time fixed using excel for han data consolidation file
</commit_message>
<xml_diff>
--- a/han/P_Pro.xlsx
+++ b/han/P_Pro.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyang/Desktop/Project-3/Project_3/han/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BE9C974-715E-6B42-A650-F9DD3301CED0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A72848-BE5C-4945-ABDF-357141C90F35}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16440"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P_Pro" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -509,10 +509,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -867,10 +866,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B560"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A330" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A616" workbookViewId="0">
+      <selection activeCell="A338" sqref="A338:A560"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3571,1784 +3572,1784 @@
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A338" s="2">
-        <v>43466</v>
+      <c r="A338" s="1">
+        <v>36892</v>
       </c>
       <c r="B338">
         <v>233137.68700000001</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A339" s="2">
-        <v>43497</v>
+      <c r="A339" s="1">
+        <v>36923</v>
       </c>
       <c r="B339">
         <v>232767.27739999999</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A340" s="2">
-        <v>43525</v>
+      <c r="A340" s="1">
+        <v>36951</v>
       </c>
       <c r="B340">
         <v>235035.66089999999</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A341" s="2">
-        <v>43556</v>
+      <c r="A341" s="1">
+        <v>36982</v>
       </c>
       <c r="B341">
         <v>231940.68179999999</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A342" s="2">
-        <v>43586</v>
+      <c r="A342" s="1">
+        <v>37012</v>
       </c>
       <c r="B342">
         <v>230059.44570000001</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A343" s="2">
-        <v>43617</v>
+      <c r="A343" s="1">
+        <v>37043</v>
       </c>
       <c r="B343">
         <v>225375.71650000001</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A344" s="2">
-        <v>43647</v>
+      <c r="A344" s="1">
+        <v>37073</v>
       </c>
       <c r="B344">
         <v>231313.7115</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A345" s="2">
-        <v>43678</v>
+      <c r="A345" s="1">
+        <v>37104</v>
       </c>
       <c r="B345">
         <v>231837.5533</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A346" s="2">
-        <v>43709</v>
+      <c r="A346" s="1">
+        <v>37135</v>
       </c>
       <c r="B346">
         <v>230517.0577</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A347" s="2">
-        <v>43739</v>
+      <c r="A347" s="1">
+        <v>37165</v>
       </c>
       <c r="B347">
         <v>230429.0111</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A348" s="2">
-        <v>43770</v>
+      <c r="A348" s="1">
+        <v>37196</v>
       </c>
       <c r="B348">
         <v>231950.21599999999</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A349" s="2">
-        <v>43800</v>
+      <c r="A349" s="1">
+        <v>37226</v>
       </c>
       <c r="B349">
         <v>229803.48050000001</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A350" s="2">
-        <v>43467</v>
+      <c r="A350" s="1">
+        <v>37257</v>
       </c>
       <c r="B350">
         <v>228186.7518</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A351" s="2">
-        <v>43498</v>
+      <c r="A351" s="1">
+        <v>37288</v>
       </c>
       <c r="B351">
         <v>228555.65349999999</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A352" s="2">
-        <v>43526</v>
+      <c r="A352" s="1">
+        <v>37316</v>
       </c>
       <c r="B352">
         <v>227922.82769999999</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A353" s="2">
-        <v>43557</v>
+      <c r="A353" s="1">
+        <v>37347</v>
       </c>
       <c r="B353">
         <v>226480.76850000001</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A354" s="2">
-        <v>43587</v>
+      <c r="A354" s="1">
+        <v>37377</v>
       </c>
       <c r="B354">
         <v>228396.2898</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A355" s="2">
-        <v>43618</v>
+      <c r="A355" s="1">
+        <v>37408</v>
       </c>
       <c r="B355">
         <v>227470.57430000001</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A356" s="2">
-        <v>43648</v>
+      <c r="A356" s="1">
+        <v>37438</v>
       </c>
       <c r="B356">
         <v>228776.50390000001</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A357" s="2">
-        <v>43679</v>
+      <c r="A357" s="1">
+        <v>37469</v>
       </c>
       <c r="B357">
         <v>228267.4872</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A358" s="2">
-        <v>43710</v>
+      <c r="A358" s="1">
+        <v>37500</v>
       </c>
       <c r="B358">
         <v>229963.81049999999</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A359" s="2">
-        <v>43740</v>
+      <c r="A359" s="1">
+        <v>37530</v>
       </c>
       <c r="B359">
         <v>234348.92009999999</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A360" s="2">
-        <v>43771</v>
+      <c r="A360" s="1">
+        <v>37561</v>
       </c>
       <c r="B360">
         <v>235145.2837</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A361" s="2">
-        <v>43801</v>
+      <c r="A361" s="1">
+        <v>37591</v>
       </c>
       <c r="B361">
         <v>229276.40520000001</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A362" s="2">
-        <v>43468</v>
+      <c r="A362" s="1">
+        <v>37622</v>
       </c>
       <c r="B362">
         <v>230655.45110000001</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A363" s="2">
-        <v>43499</v>
+      <c r="A363" s="1">
+        <v>37653</v>
       </c>
       <c r="B363">
         <v>236053.03479999999</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A364" s="2">
-        <v>43527</v>
+      <c r="A364" s="1">
+        <v>37681</v>
       </c>
       <c r="B364">
         <v>237432.73980000001</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A365" s="2">
-        <v>43558</v>
+      <c r="A365" s="1">
+        <v>37712</v>
       </c>
       <c r="B365">
         <v>234041.753</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A366" s="2">
-        <v>43588</v>
+      <c r="A366" s="1">
+        <v>37742</v>
       </c>
       <c r="B366">
         <v>233874.4725</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A367" s="2">
-        <v>43619</v>
+      <c r="A367" s="1">
+        <v>37773</v>
       </c>
       <c r="B367">
         <v>231729.6324</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A368" s="2">
-        <v>43649</v>
+      <c r="A368" s="1">
+        <v>37803</v>
       </c>
       <c r="B368">
         <v>234274.0202</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A369" s="2">
-        <v>43680</v>
+      <c r="A369" s="1">
+        <v>37834</v>
       </c>
       <c r="B369">
         <v>235877.03279999999</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A370" s="2">
-        <v>43711</v>
+      <c r="A370" s="1">
+        <v>37865</v>
       </c>
       <c r="B370">
         <v>238229.70370000001</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A371" s="2">
-        <v>43741</v>
+      <c r="A371" s="1">
+        <v>37895</v>
       </c>
       <c r="B371">
         <v>241455.64129999999</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A372" s="2">
-        <v>43772</v>
+      <c r="A372" s="1">
+        <v>37926</v>
       </c>
       <c r="B372">
         <v>242482.03109999999</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A373" s="2">
-        <v>43802</v>
+      <c r="A373" s="1">
+        <v>37956</v>
       </c>
       <c r="B373">
         <v>246384.58929999999</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A374" s="2">
-        <v>43469</v>
+      <c r="A374" s="1">
+        <v>37987</v>
       </c>
       <c r="B374">
         <v>246013.0128</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A375" s="2">
-        <v>43500</v>
+      <c r="A375" s="1">
+        <v>38018</v>
       </c>
       <c r="B375">
         <v>246035.53159999999</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A376" s="2">
-        <v>43528</v>
+      <c r="A376" s="1">
+        <v>38047</v>
       </c>
       <c r="B376">
         <v>245765.5496</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A377" s="2">
-        <v>43559</v>
+      <c r="A377" s="1">
+        <v>38078</v>
       </c>
       <c r="B377">
         <v>245367.0491</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A378" s="2">
-        <v>43589</v>
+      <c r="A378" s="1">
+        <v>38108</v>
       </c>
       <c r="B378">
         <v>244097.18719999999</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A379" s="2">
-        <v>43620</v>
+      <c r="A379" s="1">
+        <v>38139</v>
       </c>
       <c r="B379">
         <v>249082.82879999999</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A380" s="2">
-        <v>43650</v>
+      <c r="A380" s="1">
+        <v>38169</v>
       </c>
       <c r="B380">
         <v>250922.3578</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A381" s="2">
-        <v>43681</v>
+      <c r="A381" s="1">
+        <v>38200</v>
       </c>
       <c r="B381">
         <v>247692.6</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A382" s="2">
-        <v>43712</v>
+      <c r="A382" s="1">
+        <v>38231</v>
       </c>
       <c r="B382">
         <v>249442.45740000001</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A383" s="2">
-        <v>43742</v>
+      <c r="A383" s="1">
+        <v>38261</v>
       </c>
       <c r="B383">
         <v>252060.03570000001</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A384" s="2">
-        <v>43773</v>
+      <c r="A384" s="1">
+        <v>38292</v>
       </c>
       <c r="B384">
         <v>251506.66560000001</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A385" s="2">
-        <v>43803</v>
+      <c r="A385" s="1">
+        <v>38322</v>
       </c>
       <c r="B385">
         <v>250492.6728</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A386" s="2">
-        <v>43470</v>
+      <c r="A386" s="1">
+        <v>38353</v>
       </c>
       <c r="B386">
         <v>251644.46</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A387" s="2">
-        <v>43501</v>
+      <c r="A387" s="1">
+        <v>38384</v>
       </c>
       <c r="B387">
         <v>252807.96299999999</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A388" s="2">
-        <v>43529</v>
+      <c r="A388" s="1">
+        <v>38412</v>
       </c>
       <c r="B388">
         <v>253257.48800000001</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A389" s="2">
-        <v>43560</v>
+      <c r="A389" s="1">
+        <v>38443</v>
       </c>
       <c r="B389">
         <v>254515.81599999999</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A390" s="2">
-        <v>43590</v>
+      <c r="A390" s="1">
+        <v>38473</v>
       </c>
       <c r="B390">
         <v>255410.41699999999</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A391" s="2">
-        <v>43621</v>
+      <c r="A391" s="1">
+        <v>38504</v>
       </c>
       <c r="B391">
         <v>253969.647</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A392" s="2">
-        <v>43651</v>
+      <c r="A392" s="1">
+        <v>38534</v>
       </c>
       <c r="B392">
         <v>253052.166</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A393" s="2">
-        <v>43682</v>
+      <c r="A393" s="1">
+        <v>38565</v>
       </c>
       <c r="B393">
         <v>253743.11</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A394" s="2">
-        <v>43713</v>
+      <c r="A394" s="1">
+        <v>38596</v>
       </c>
       <c r="B394">
         <v>251696.935</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A395" s="2">
-        <v>43743</v>
+      <c r="A395" s="1">
+        <v>38626</v>
       </c>
       <c r="B395">
         <v>251641.432</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A396" s="2">
-        <v>43774</v>
+      <c r="A396" s="1">
+        <v>38657</v>
       </c>
       <c r="B396">
         <v>254021.524</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A397" s="2">
-        <v>43804</v>
+      <c r="A397" s="1">
+        <v>38687</v>
       </c>
       <c r="B397">
         <v>253142.79500000001</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A398" s="2">
-        <v>43471</v>
+      <c r="A398" s="1">
+        <v>38718</v>
       </c>
       <c r="B398">
         <v>253010.58199999999</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A399" s="2">
-        <v>43502</v>
+      <c r="A399" s="1">
+        <v>38749</v>
       </c>
       <c r="B399">
         <v>253162.269</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A400" s="2">
-        <v>43530</v>
+      <c r="A400" s="1">
+        <v>38777</v>
       </c>
       <c r="B400">
         <v>252072.64300000001</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A401" s="2">
-        <v>43561</v>
+      <c r="A401" s="1">
+        <v>38808</v>
       </c>
       <c r="B401">
         <v>252987.37</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A402" s="2">
-        <v>43591</v>
+      <c r="A402" s="1">
+        <v>38838</v>
       </c>
       <c r="B402">
         <v>252335.55799999999</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A403" s="2">
-        <v>43622</v>
+      <c r="A403" s="1">
+        <v>38869</v>
       </c>
       <c r="B403">
         <v>252296.902</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A404" s="2">
-        <v>43652</v>
+      <c r="A404" s="1">
+        <v>38899</v>
       </c>
       <c r="B404">
         <v>256282.52900000001</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A405" s="2">
-        <v>43683</v>
+      <c r="A405" s="1">
+        <v>38930</v>
       </c>
       <c r="B405">
         <v>255642.32199999999</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A406" s="2">
-        <v>43714</v>
+      <c r="A406" s="1">
+        <v>38961</v>
       </c>
       <c r="B406">
         <v>254137.16500000001</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A407" s="2">
-        <v>43744</v>
+      <c r="A407" s="1">
+        <v>38991</v>
       </c>
       <c r="B407">
         <v>254936.46100000001</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A408" s="2">
-        <v>43775</v>
+      <c r="A408" s="1">
+        <v>39022</v>
       </c>
       <c r="B408">
         <v>253378.228</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A409" s="2">
-        <v>43805</v>
+      <c r="A409" s="1">
+        <v>39052</v>
       </c>
       <c r="B409">
         <v>252543.87299999999</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A410" s="2">
-        <v>43472</v>
+      <c r="A410" s="1">
+        <v>39083</v>
       </c>
       <c r="B410">
         <v>251945.11799999999</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A411" s="2">
-        <v>43503</v>
+      <c r="A411" s="1">
+        <v>39114</v>
       </c>
       <c r="B411">
         <v>252833.723</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A412" s="2">
-        <v>43531</v>
+      <c r="A412" s="1">
+        <v>39142</v>
       </c>
       <c r="B412">
         <v>252475.67499999999</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A413" s="2">
-        <v>43562</v>
+      <c r="A413" s="1">
+        <v>39173</v>
       </c>
       <c r="B413">
         <v>253734.75399999999</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A414" s="2">
-        <v>43592</v>
+      <c r="A414" s="1">
+        <v>39203</v>
       </c>
       <c r="B414">
         <v>252705.10500000001</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A415" s="2">
-        <v>43623</v>
+      <c r="A415" s="1">
+        <v>39234</v>
       </c>
       <c r="B415">
         <v>252607.10200000001</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A416" s="2">
-        <v>43653</v>
+      <c r="A416" s="1">
+        <v>39264</v>
       </c>
       <c r="B416">
         <v>254023.47</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A417" s="2">
-        <v>43684</v>
+      <c r="A417" s="1">
+        <v>39295</v>
       </c>
       <c r="B417">
         <v>251607.16200000001</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A418" s="2">
-        <v>43715</v>
+      <c r="A418" s="1">
+        <v>39326</v>
       </c>
       <c r="B418">
         <v>254140.753</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A419" s="2">
-        <v>43745</v>
+      <c r="A419" s="1">
+        <v>39356</v>
       </c>
       <c r="B419">
         <v>256396.459</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A420" s="2">
-        <v>43776</v>
+      <c r="A420" s="1">
+        <v>39387</v>
       </c>
       <c r="B420">
         <v>255667.25899999999</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A421" s="2">
-        <v>43806</v>
+      <c r="A421" s="1">
+        <v>39417</v>
       </c>
       <c r="B421">
         <v>257167.405</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A422" s="2">
-        <v>43473</v>
+      <c r="A422" s="1">
+        <v>39448</v>
       </c>
       <c r="B422">
         <v>257231.59899999999</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A423" s="2">
-        <v>43504</v>
+      <c r="A423" s="1">
+        <v>39479</v>
       </c>
       <c r="B423">
         <v>257570.519</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A424" s="2">
-        <v>43532</v>
+      <c r="A424" s="1">
+        <v>39508</v>
       </c>
       <c r="B424">
         <v>258275.59400000001</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A425" s="2">
-        <v>43563</v>
+      <c r="A425" s="1">
+        <v>39539</v>
       </c>
       <c r="B425">
         <v>256841.33900000001</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A426" s="2">
-        <v>43593</v>
+      <c r="A426" s="1">
+        <v>39569</v>
       </c>
       <c r="B426">
         <v>258924.41200000001</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A427" s="2">
-        <v>43624</v>
+      <c r="A427" s="1">
+        <v>39600</v>
       </c>
       <c r="B427">
         <v>258841.19899999999</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A428" s="2">
-        <v>43654</v>
+      <c r="A428" s="1">
+        <v>39630</v>
       </c>
       <c r="B428">
         <v>261792.978</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A429" s="2">
-        <v>43685</v>
+      <c r="A429" s="1">
+        <v>39661</v>
       </c>
       <c r="B429">
         <v>258970.10800000001</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A430" s="2">
-        <v>43716</v>
+      <c r="A430" s="1">
+        <v>39692</v>
       </c>
       <c r="B430">
         <v>254213.291</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A431" s="2">
-        <v>43746</v>
+      <c r="A431" s="1">
+        <v>39722</v>
       </c>
       <c r="B431">
         <v>258829.715</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A432" s="2">
-        <v>43777</v>
+      <c r="A432" s="1">
+        <v>39753</v>
       </c>
       <c r="B432">
         <v>258066.49</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A433" s="2">
-        <v>43807</v>
+      <c r="A433" s="1">
+        <v>39783</v>
       </c>
       <c r="B433">
         <v>254218.304</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A434" s="2">
-        <v>43474</v>
+      <c r="A434" s="1">
+        <v>39814</v>
       </c>
       <c r="B434">
         <v>250975.046</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A435" s="2">
-        <v>43505</v>
+      <c r="A435" s="1">
+        <v>39845</v>
       </c>
       <c r="B435">
         <v>252987.698</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A436" s="2">
-        <v>43533</v>
+      <c r="A436" s="1">
+        <v>39873</v>
       </c>
       <c r="B436">
         <v>252705.19399999999</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A437" s="2">
-        <v>43564</v>
+      <c r="A437" s="1">
+        <v>39904</v>
       </c>
       <c r="B437">
         <v>253819.14</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A438" s="2">
-        <v>43594</v>
+      <c r="A438" s="1">
+        <v>39934</v>
       </c>
       <c r="B438">
         <v>253667.86</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A439" s="2">
-        <v>43625</v>
+      <c r="A439" s="1">
+        <v>39965</v>
       </c>
       <c r="B439">
         <v>254493.261</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A440" s="2">
-        <v>43655</v>
+      <c r="A440" s="1">
+        <v>39995</v>
       </c>
       <c r="B440">
         <v>257001.429</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A441" s="2">
-        <v>43686</v>
+      <c r="A441" s="1">
+        <v>40026</v>
       </c>
       <c r="B441">
         <v>255965.87899999999</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A442" s="2">
-        <v>43717</v>
+      <c r="A442" s="1">
+        <v>40057</v>
       </c>
       <c r="B442">
         <v>257195.16099999999</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A443" s="2">
-        <v>43747</v>
+      <c r="A443" s="1">
+        <v>40087</v>
       </c>
       <c r="B443">
         <v>258607.98199999999</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A444" s="2">
-        <v>43778</v>
+      <c r="A444" s="1">
+        <v>40118</v>
       </c>
       <c r="B444">
         <v>259041.85200000001</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A445" s="2">
-        <v>43808</v>
+      <c r="A445" s="1">
+        <v>40148</v>
       </c>
       <c r="B445">
         <v>257534.74799999999</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A446" s="2">
-        <v>43475</v>
+      <c r="A446" s="1">
+        <v>40179</v>
       </c>
       <c r="B446">
         <v>258645.46299999999</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A447" s="2">
-        <v>43506</v>
+      <c r="A447" s="1">
+        <v>40210</v>
       </c>
       <c r="B447">
         <v>260379.49799999999</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A448" s="2">
-        <v>43534</v>
+      <c r="A448" s="1">
+        <v>40238</v>
       </c>
       <c r="B448">
         <v>261508.05900000001</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A449" s="2">
-        <v>43565</v>
+      <c r="A449" s="1">
+        <v>40269</v>
       </c>
       <c r="B449">
         <v>262426.19900000002</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A450" s="2">
-        <v>43595</v>
+      <c r="A450" s="1">
+        <v>40299</v>
       </c>
       <c r="B450">
         <v>263637.08799999999</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A451" s="2">
-        <v>43626</v>
+      <c r="A451" s="1">
+        <v>40330</v>
       </c>
       <c r="B451">
         <v>263969.41899999999</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A452" s="2">
-        <v>43656</v>
+      <c r="A452" s="1">
+        <v>40360</v>
       </c>
       <c r="B452">
         <v>264724.06300000002</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A453" s="2">
-        <v>43687</v>
+      <c r="A453" s="1">
+        <v>40391</v>
       </c>
       <c r="B453">
         <v>264452.12099999998</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A454" s="2">
-        <v>43718</v>
+      <c r="A454" s="1">
+        <v>40422</v>
       </c>
       <c r="B454">
         <v>265001.11900000001</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A455" s="2">
-        <v>43748</v>
+      <c r="A455" s="1">
+        <v>40452</v>
       </c>
       <c r="B455">
         <v>264403.70899999997</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A456" s="2">
-        <v>43779</v>
+      <c r="A456" s="1">
+        <v>40483</v>
       </c>
       <c r="B456">
         <v>265766.28600000002</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A457" s="2">
-        <v>43809</v>
+      <c r="A457" s="1">
+        <v>40513</v>
       </c>
       <c r="B457">
         <v>265209.66399999999</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A458" s="2">
-        <v>43476</v>
+      <c r="A458" s="1">
+        <v>40544</v>
       </c>
       <c r="B458">
         <v>267452.67</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A459" s="2">
-        <v>43507</v>
+      <c r="A459" s="1">
+        <v>40575</v>
       </c>
       <c r="B459">
         <v>264061.17499999999</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A460" s="2">
-        <v>43535</v>
+      <c r="A460" s="1">
+        <v>40603</v>
       </c>
       <c r="B460">
         <v>261344.43299999999</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A461" s="2">
-        <v>43566</v>
+      <c r="A461" s="1">
+        <v>40634</v>
       </c>
       <c r="B461">
         <v>261170.67800000001</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A462" s="2">
-        <v>43596</v>
+      <c r="A462" s="1">
+        <v>40664</v>
       </c>
       <c r="B462">
         <v>260615.92600000001</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A463" s="2">
-        <v>43627</v>
+      <c r="A463" s="1">
+        <v>40695</v>
       </c>
       <c r="B463">
         <v>263343.55699999997</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A464" s="2">
-        <v>43657</v>
+      <c r="A464" s="1">
+        <v>40725</v>
       </c>
       <c r="B464">
         <v>264752.94699999999</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A465" s="2">
-        <v>43688</v>
+      <c r="A465" s="1">
+        <v>40756</v>
       </c>
       <c r="B465">
         <v>266250.33600000001</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A466" s="2">
-        <v>43719</v>
+      <c r="A466" s="1">
+        <v>40787</v>
       </c>
       <c r="B466">
         <v>264093.52</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A467" s="2">
-        <v>43749</v>
+      <c r="A467" s="1">
+        <v>40817</v>
       </c>
       <c r="B467">
         <v>265439.38799999998</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A468" s="2">
-        <v>43780</v>
+      <c r="A468" s="1">
+        <v>40848</v>
       </c>
       <c r="B468">
         <v>268440.99</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A469" s="2">
-        <v>43810</v>
+      <c r="A469" s="1">
+        <v>40878</v>
       </c>
       <c r="B469">
         <v>269371.48499999999</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A470" s="2">
-        <v>43477</v>
+      <c r="A470" s="1">
+        <v>40909</v>
       </c>
       <c r="B470">
         <v>269775.37599999999</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A471" s="2">
-        <v>43508</v>
+      <c r="A471" s="1">
+        <v>40940</v>
       </c>
       <c r="B471">
         <v>271319.09700000001</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A472" s="2">
-        <v>43536</v>
+      <c r="A472" s="1">
+        <v>40969</v>
       </c>
       <c r="B472">
         <v>270345.79300000001</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A473" s="2">
-        <v>43567</v>
+      <c r="A473" s="1">
+        <v>41000</v>
       </c>
       <c r="B473">
         <v>271572.96600000001</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A474" s="2">
-        <v>43597</v>
+      <c r="A474" s="1">
+        <v>41030</v>
       </c>
       <c r="B474">
         <v>270317.29499999998</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A475" s="2">
-        <v>43628</v>
+      <c r="A475" s="1">
+        <v>41061</v>
       </c>
       <c r="B475">
         <v>269508.52399999998</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A476" s="2">
-        <v>43658</v>
+      <c r="A476" s="1">
+        <v>41091</v>
       </c>
       <c r="B476">
         <v>270836.79800000001</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A477" s="2">
-        <v>43689</v>
+      <c r="A477" s="1">
+        <v>41122</v>
       </c>
       <c r="B477">
         <v>271115.44500000001</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A478" s="2">
-        <v>43720</v>
+      <c r="A478" s="1">
+        <v>41153</v>
       </c>
       <c r="B478">
         <v>269054.10600000003</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A479" s="2">
-        <v>43750</v>
+      <c r="A479" s="1">
+        <v>41183</v>
       </c>
       <c r="B479">
         <v>271206.03600000002</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A480" s="2">
-        <v>43781</v>
+      <c r="A480" s="1">
+        <v>41214</v>
       </c>
       <c r="B480">
         <v>272651.37199999997</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A481" s="2">
-        <v>43811</v>
+      <c r="A481" s="1">
+        <v>41244</v>
       </c>
       <c r="B481">
         <v>271611.40100000001</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A482" s="2">
-        <v>43478</v>
+      <c r="A482" s="1">
+        <v>41275</v>
       </c>
       <c r="B482">
         <v>269284.11900000001</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A483" s="2">
-        <v>43509</v>
+      <c r="A483" s="1">
+        <v>41306</v>
       </c>
       <c r="B483">
         <v>268700.315</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A484" s="2">
-        <v>43537</v>
+      <c r="A484" s="1">
+        <v>41334</v>
       </c>
       <c r="B484">
         <v>269371.16800000001</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A485" s="2">
-        <v>43568</v>
+      <c r="A485" s="1">
+        <v>41365</v>
       </c>
       <c r="B485">
         <v>271931.07299999997</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A486" s="2">
-        <v>43598</v>
+      <c r="A486" s="1">
+        <v>41395</v>
       </c>
       <c r="B486">
         <v>272223.63099999999</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A487" s="2">
-        <v>43629</v>
+      <c r="A487" s="1">
+        <v>41426</v>
       </c>
       <c r="B487">
         <v>272176.054</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A488" s="2">
-        <v>43659</v>
+      <c r="A488" s="1">
+        <v>41456</v>
       </c>
       <c r="B488">
         <v>274724.71500000003</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A489" s="2">
-        <v>43690</v>
+      <c r="A489" s="1">
+        <v>41487</v>
       </c>
       <c r="B489">
         <v>274335.51899999997</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A490" s="2">
-        <v>43721</v>
+      <c r="A490" s="1">
+        <v>41518</v>
       </c>
       <c r="B490">
         <v>272350.41200000001</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A491" s="2">
-        <v>43751</v>
+      <c r="A491" s="1">
+        <v>41548</v>
       </c>
       <c r="B491">
         <v>273115.185</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A492" s="2">
-        <v>43782</v>
+      <c r="A492" s="1">
+        <v>41579</v>
       </c>
       <c r="B492">
         <v>273950.31800000003</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A493" s="2">
-        <v>43812</v>
+      <c r="A493" s="1">
+        <v>41609</v>
       </c>
       <c r="B493">
         <v>274238.33899999998</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A494" s="2">
-        <v>43479</v>
+      <c r="A494" s="1">
+        <v>41640</v>
       </c>
       <c r="B494">
         <v>274616.21999999997</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A495" s="2">
-        <v>43510</v>
+      <c r="A495" s="1">
+        <v>41671</v>
       </c>
       <c r="B495">
         <v>276229.41899999999</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A496" s="2">
-        <v>43538</v>
+      <c r="A496" s="1">
+        <v>41699</v>
       </c>
       <c r="B496">
         <v>274747.45199999999</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A497" s="2">
-        <v>43569</v>
+      <c r="A497" s="1">
+        <v>41730</v>
       </c>
       <c r="B497">
         <v>275404.57900000003</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A498" s="2">
-        <v>43599</v>
+      <c r="A498" s="1">
+        <v>41760</v>
       </c>
       <c r="B498">
         <v>276738.28000000003</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A499" s="2">
-        <v>43630</v>
+      <c r="A499" s="1">
+        <v>41791</v>
       </c>
       <c r="B499">
         <v>279152.92599999998</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A500" s="2">
-        <v>43660</v>
+      <c r="A500" s="1">
+        <v>41821</v>
       </c>
       <c r="B500">
         <v>279735.96899999998</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A501" s="2">
-        <v>43691</v>
+      <c r="A501" s="1">
+        <v>41852</v>
       </c>
       <c r="B501">
         <v>280945.23499999999</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A502" s="2">
-        <v>43722</v>
+      <c r="A502" s="1">
+        <v>41883</v>
       </c>
       <c r="B502">
         <v>282668.12099999998</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A503" s="2">
-        <v>43752</v>
+      <c r="A503" s="1">
+        <v>41913</v>
       </c>
       <c r="B503">
         <v>286208.99099999998</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A504" s="2">
-        <v>43783</v>
+      <c r="A504" s="1">
+        <v>41944</v>
       </c>
       <c r="B504">
         <v>284521.36200000002</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A505" s="2">
-        <v>43813</v>
+      <c r="A505" s="1">
+        <v>41974</v>
       </c>
       <c r="B505">
         <v>286782.77100000001</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A506" s="2">
-        <v>43480</v>
+      <c r="A506" s="1">
+        <v>42005</v>
       </c>
       <c r="B506">
         <v>283394.15999999997</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A507" s="2">
-        <v>43511</v>
+      <c r="A507" s="1">
+        <v>42036</v>
       </c>
       <c r="B507">
         <v>283112.19</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A508" s="2">
-        <v>43539</v>
+      <c r="A508" s="1">
+        <v>42064</v>
       </c>
       <c r="B508">
         <v>286303.74599999998</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A509" s="2">
-        <v>43570</v>
+      <c r="A509" s="1">
+        <v>42095</v>
       </c>
       <c r="B509">
         <v>286483.84499999997</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A510" s="2">
-        <v>43600</v>
+      <c r="A510" s="1">
+        <v>42125</v>
       </c>
       <c r="B510">
         <v>287245.41499999998</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A511" s="2">
-        <v>43631</v>
+      <c r="A511" s="1">
+        <v>42156</v>
       </c>
       <c r="B511">
         <v>288889.29499999998</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A512" s="2">
-        <v>43661</v>
+      <c r="A512" s="1">
+        <v>42186</v>
       </c>
       <c r="B512">
         <v>290566.85800000001</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A513" s="2">
-        <v>43692</v>
+      <c r="A513" s="1">
+        <v>42217</v>
       </c>
       <c r="B513">
         <v>290334.31599999999</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A514" s="2">
-        <v>43723</v>
+      <c r="A514" s="1">
+        <v>42248</v>
       </c>
       <c r="B514">
         <v>289666.30200000003</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A515" s="2">
-        <v>43753</v>
+      <c r="A515" s="1">
+        <v>42278</v>
       </c>
       <c r="B515">
         <v>290281.66899999999</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A516" s="2">
-        <v>43784</v>
+      <c r="A516" s="1">
+        <v>42309</v>
       </c>
       <c r="B516">
         <v>291112.31</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A517" s="2">
-        <v>43814</v>
+      <c r="A517" s="1">
+        <v>42339</v>
       </c>
       <c r="B517">
         <v>290975.61800000002</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A518" s="2">
-        <v>43481</v>
+      <c r="A518" s="1">
+        <v>42370</v>
       </c>
       <c r="B518">
         <v>290455.804</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A519" s="2">
-        <v>43512</v>
+      <c r="A519" s="1">
+        <v>42401</v>
       </c>
       <c r="B519">
         <v>287923.56199999998</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A520" s="2">
-        <v>43540</v>
+      <c r="A520" s="1">
+        <v>42430</v>
       </c>
       <c r="B520">
         <v>288423.77100000001</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A521" s="2">
-        <v>43571</v>
+      <c r="A521" s="1">
+        <v>42461</v>
       </c>
       <c r="B521">
         <v>287446.37199999997</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A522" s="2">
-        <v>43601</v>
+      <c r="A522" s="1">
+        <v>42491</v>
       </c>
       <c r="B522">
         <v>285931.67300000001</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A523" s="2">
-        <v>43632</v>
+      <c r="A523" s="1">
+        <v>42522</v>
       </c>
       <c r="B523">
         <v>287438.83</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A524" s="2">
-        <v>43662</v>
+      <c r="A524" s="1">
+        <v>42552</v>
       </c>
       <c r="B524">
         <v>290606.12699999998</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A525" s="2">
-        <v>43693</v>
+      <c r="A525" s="1">
+        <v>42583</v>
       </c>
       <c r="B525">
         <v>287620.66200000001</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A526" s="2">
-        <v>43724</v>
+      <c r="A526" s="1">
+        <v>42614</v>
       </c>
       <c r="B526">
         <v>288073.25799999997</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A527" s="2">
-        <v>43754</v>
+      <c r="A527" s="1">
+        <v>42644</v>
       </c>
       <c r="B527">
         <v>291784.47100000002</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A528" s="2">
-        <v>43785</v>
+      <c r="A528" s="1">
+        <v>42675</v>
       </c>
       <c r="B528">
         <v>295191.32400000002</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A529" s="2">
-        <v>43815</v>
+      <c r="A529" s="1">
+        <v>42705</v>
       </c>
       <c r="B529">
         <v>291927.67499999999</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A530" s="2">
-        <v>43482</v>
+      <c r="A530" s="1">
+        <v>42736</v>
       </c>
       <c r="B530">
         <v>288973.02799999999</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A531" s="2">
-        <v>43513</v>
+      <c r="A531" s="1">
+        <v>42767</v>
       </c>
       <c r="B531">
         <v>289429.136</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A532" s="2">
-        <v>43541</v>
+      <c r="A532" s="1">
+        <v>42795</v>
       </c>
       <c r="B532">
         <v>287497.239</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A533" s="2">
-        <v>43572</v>
+      <c r="A533" s="1">
+        <v>42826</v>
       </c>
       <c r="B533">
         <v>286877.55</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A534" s="2">
-        <v>43602</v>
+      <c r="A534" s="1">
+        <v>42856</v>
       </c>
       <c r="B534">
         <v>289741.71999999997</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A535" s="2">
-        <v>43633</v>
+      <c r="A535" s="1">
+        <v>42887</v>
       </c>
       <c r="B535">
         <v>291875.41499999998</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A536" s="2">
-        <v>43663</v>
+      <c r="A536" s="1">
+        <v>42917</v>
       </c>
       <c r="B536">
         <v>294037.90000000002</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A537" s="2">
-        <v>43694</v>
+      <c r="A537" s="1">
+        <v>42948</v>
       </c>
       <c r="B537">
         <v>291783.83899999998</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A538" s="2">
-        <v>43725</v>
+      <c r="A538" s="1">
+        <v>42979</v>
       </c>
       <c r="B538">
         <v>292217.81800000003</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A539" s="2">
-        <v>43755</v>
+      <c r="A539" s="1">
+        <v>43009</v>
       </c>
       <c r="B539">
         <v>293700.46799999999</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A540" s="2">
-        <v>43786</v>
+      <c r="A540" s="1">
+        <v>43040</v>
       </c>
       <c r="B540">
         <v>295432.24300000002</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A541" s="2">
-        <v>43816</v>
+      <c r="A541" s="1">
+        <v>43070</v>
       </c>
       <c r="B541">
         <v>293199.71799999999</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A542" s="2">
-        <v>43483</v>
+      <c r="A542" s="1">
+        <v>43101</v>
       </c>
       <c r="B542">
         <v>294525.3</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A543" s="2">
-        <v>43514</v>
+      <c r="A543" s="1">
+        <v>43132</v>
       </c>
       <c r="B543">
         <v>295367.56199999998</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A544" s="2">
-        <v>43542</v>
+      <c r="A544" s="1">
+        <v>43160</v>
       </c>
       <c r="B544">
         <v>295706.09000000003</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A545" s="2">
-        <v>43573</v>
+      <c r="A545" s="1">
+        <v>43191</v>
       </c>
       <c r="B545">
         <v>295885.005</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A546" s="2">
-        <v>43603</v>
+      <c r="A546" s="1">
+        <v>43221</v>
       </c>
       <c r="B546">
         <v>295849.44300000003</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A547" s="2">
-        <v>43634</v>
+      <c r="A547" s="1">
+        <v>43252</v>
       </c>
       <c r="B547">
         <v>298371.65600000002</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A548" s="2">
-        <v>43664</v>
+      <c r="A548" s="1">
+        <v>43282</v>
       </c>
       <c r="B548">
         <v>300698.80099999998</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A549" s="2">
-        <v>43695</v>
+      <c r="A549" s="1">
+        <v>43313</v>
       </c>
       <c r="B549">
         <v>302101.64</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A550" s="2">
-        <v>43726</v>
+      <c r="A550" s="1">
+        <v>43344</v>
       </c>
       <c r="B550">
         <v>302215.07699999999</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A551" s="2">
-        <v>43756</v>
+      <c r="A551" s="1">
+        <v>43374</v>
       </c>
       <c r="B551">
         <v>304741.65500000003</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A552" s="2">
-        <v>43787</v>
+      <c r="A552" s="1">
+        <v>43405</v>
       </c>
       <c r="B552">
         <v>305019.179</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A553" s="2">
-        <v>43817</v>
+      <c r="A553" s="1">
+        <v>43435</v>
       </c>
       <c r="B553">
         <v>303033.66399999999</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A554" s="2">
-        <v>43484</v>
+      <c r="A554" s="1">
+        <v>43466</v>
       </c>
       <c r="B554">
         <v>298683.28399999999</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A555" s="2">
-        <v>43515</v>
+      <c r="A555" s="1">
+        <v>43497</v>
       </c>
       <c r="B555">
         <v>298063.44099999999</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A556" s="2">
-        <v>43543</v>
+      <c r="A556" s="1">
+        <v>43525</v>
       </c>
       <c r="B556">
         <v>298013.62300000002</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A557" s="2">
-        <v>43574</v>
+      <c r="A557" s="1">
+        <v>43556</v>
       </c>
       <c r="B557">
         <v>298315.38299999997</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A558" s="2">
-        <v>43604</v>
+      <c r="A558" s="1">
+        <v>43586</v>
       </c>
       <c r="B558">
         <v>297656.18099999998</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A559" s="2">
-        <v>43635</v>
+      <c r="A559" s="1">
+        <v>43617</v>
       </c>
       <c r="B559">
         <v>298811.56800000003</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A560" s="2">
-        <v>43665</v>
+      <c r="A560" s="1">
+        <v>43647</v>
       </c>
       <c r="B560">
         <v>297266.93199999997</v>

</xml_diff>